<commit_message>
Update PS table menu v1_2_0
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0.xlsx
+++ b/development/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_2_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E080DC35-1F73-C047-B49F-C9BA7A013BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CFCBE7-62B5-FE49-A737-DB3C8664D72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1247,7 +1247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1259,6 +1259,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1296,11 +1303,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1605,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K397"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="E335" sqref="E335"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13248,25 +13256,25 @@
         <v>0</v>
       </c>
       <c r="E333">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F333">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G333">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H333">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I333">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J333">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K333">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="334" spans="1:11" x14ac:dyDescent="0.2">
@@ -13283,25 +13291,25 @@
         <v>0</v>
       </c>
       <c r="E334">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F334">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G334">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H334">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I334">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J334">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K334">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="335" spans="1:11" x14ac:dyDescent="0.2">
@@ -13318,25 +13326,25 @@
         <v>0</v>
       </c>
       <c r="E335">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F335">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G335">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H335">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I335">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J335">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K335">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="336" spans="1:11" x14ac:dyDescent="0.2">
@@ -13559,29 +13567,29 @@
       <c r="C342">
         <v>0</v>
       </c>
-      <c r="D342">
-        <v>0</v>
-      </c>
-      <c r="E342">
-        <v>0</v>
-      </c>
-      <c r="F342">
-        <v>0</v>
-      </c>
-      <c r="G342">
-        <v>0</v>
-      </c>
-      <c r="H342">
-        <v>0</v>
-      </c>
-      <c r="I342">
-        <v>0</v>
-      </c>
-      <c r="J342">
-        <v>0</v>
-      </c>
-      <c r="K342">
-        <v>0</v>
+      <c r="D342" s="2">
+        <v>0</v>
+      </c>
+      <c r="E342" s="2">
+        <v>1</v>
+      </c>
+      <c r="F342" s="2">
+        <v>1</v>
+      </c>
+      <c r="G342" s="2">
+        <v>1</v>
+      </c>
+      <c r="H342" s="2">
+        <v>1</v>
+      </c>
+      <c r="I342" s="2">
+        <v>1</v>
+      </c>
+      <c r="J342" s="2">
+        <v>1</v>
+      </c>
+      <c r="K342" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="343" spans="1:11" x14ac:dyDescent="0.2">
@@ -13594,29 +13602,29 @@
       <c r="C343">
         <v>0</v>
       </c>
-      <c r="D343">
-        <v>0</v>
-      </c>
-      <c r="E343">
-        <v>0</v>
-      </c>
-      <c r="F343">
-        <v>0</v>
-      </c>
-      <c r="G343">
-        <v>0</v>
-      </c>
-      <c r="H343">
-        <v>0</v>
-      </c>
-      <c r="I343">
-        <v>0</v>
-      </c>
-      <c r="J343">
-        <v>0</v>
-      </c>
-      <c r="K343">
-        <v>0</v>
+      <c r="D343" s="2">
+        <v>0</v>
+      </c>
+      <c r="E343" s="2">
+        <v>1</v>
+      </c>
+      <c r="F343" s="2">
+        <v>1</v>
+      </c>
+      <c r="G343" s="2">
+        <v>1</v>
+      </c>
+      <c r="H343" s="2">
+        <v>1</v>
+      </c>
+      <c r="I343" s="2">
+        <v>1</v>
+      </c>
+      <c r="J343" s="2">
+        <v>1</v>
+      </c>
+      <c r="K343" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="344" spans="1:11" x14ac:dyDescent="0.2">
@@ -13629,29 +13637,29 @@
       <c r="C344">
         <v>0</v>
       </c>
-      <c r="D344">
-        <v>0</v>
-      </c>
-      <c r="E344">
-        <v>0</v>
-      </c>
-      <c r="F344">
-        <v>0</v>
-      </c>
-      <c r="G344">
-        <v>0</v>
-      </c>
-      <c r="H344">
-        <v>0</v>
-      </c>
-      <c r="I344">
-        <v>0</v>
-      </c>
-      <c r="J344">
-        <v>0</v>
-      </c>
-      <c r="K344">
-        <v>0</v>
+      <c r="D344" s="2">
+        <v>0</v>
+      </c>
+      <c r="E344" s="2">
+        <v>1</v>
+      </c>
+      <c r="F344" s="2">
+        <v>1</v>
+      </c>
+      <c r="G344" s="2">
+        <v>1</v>
+      </c>
+      <c r="H344" s="2">
+        <v>1</v>
+      </c>
+      <c r="I344" s="2">
+        <v>1</v>
+      </c>
+      <c r="J344" s="2">
+        <v>1</v>
+      </c>
+      <c r="K344" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Switched ON "L1_DoubleMu18er2p1_SQ" seed
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0.xlsx
+++ b/development/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_2_0/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2041462A-D3B1-344C-8A00-59EEF0123EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5AA193-6E04-1C4F-8F37-170F2D96DA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1259,6 +1259,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1614,7 +1615,7 @@
   <dimension ref="A1:K397"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3313,28 +3314,28 @@
         <v>0</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>